<commit_message>
Modify: Example input file format;
</commit_message>
<xml_diff>
--- a/assets/exampleInputFile/合併數位課綱資料/數位課綱.xlsx
+++ b/assets/exampleInputFile/合併數位課綱資料/數位課綱.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Go\src\TRC\assets\exampleXLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Go\src\github.com\vincent87720\TRC\assets\exampleInputFile\合併數位課綱資料\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="10050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7515"/>
   </bookViews>
   <sheets>
     <sheet name="工作表" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="67">
   <si>
     <t>無教師影像及聲音</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -213,13 +213,35 @@
   </si>
   <si>
     <t>杜星謙</t>
+  </si>
+  <si>
+    <t>所屬單位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>護理學系</t>
+  </si>
+  <si>
+    <t>共同教學中心</t>
+  </si>
+  <si>
+    <t>材料科學與工程學系</t>
+  </si>
+  <si>
+    <t>食品暨應用生物科技學系</t>
+  </si>
+  <si>
+    <t>環境工程學系</t>
+  </si>
+  <si>
+    <t>國際企業管理學系</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -236,10 +258,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="微軟正黑體 Light"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="微軟正黑體 Light"/>
+      <family val="2"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="2">
@@ -250,25 +280,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -277,17 +294,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -570,759 +590,918 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.875" customWidth="1"/>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
-    <col min="3" max="3" width="29.875" customWidth="1"/>
-    <col min="4" max="4" width="21.875" customWidth="1"/>
+    <col min="1" max="2" width="12.875" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="29.875" customWidth="1"/>
+    <col min="5" max="5" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="2">
         <v>73</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="2">
         <v>75</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="2">
         <v>81</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="2">
         <v>83</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="2">
         <v>1693</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="2">
         <v>1695</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="2">
         <v>1697</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="2">
         <v>1653</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="E9" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="2">
         <v>1655</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="E10" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="2">
         <v>1661</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="E11" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="2">
         <v>1665</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="E12" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="2">
         <v>1667</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="2">
         <v>1669</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="E14" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="2">
         <v>1709</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="E15" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="2">
         <v>1713</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="E16" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="2">
         <v>93</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="E17" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="2">
         <v>95</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="E18" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="2">
         <v>97</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="E19" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="2">
         <v>99</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="E20" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="2">
         <v>101</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="E21" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="2">
         <v>103</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="E22" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="2">
         <v>1645</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="E23" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="2">
         <v>1647</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="2">
         <v>1651</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="E25" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="2">
         <v>1687</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D26" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="E26" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="2">
         <v>1689</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="E27" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="2">
         <v>91</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D28" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="E28" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="2">
         <v>1715</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="E29" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="2">
         <v>1649</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D30" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="E30" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="2">
         <v>1657</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="E31" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="2">
         <v>1659</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="2">
         <v>1663</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D33" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="E33" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="2">
         <v>1671</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="E34" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="2">
         <v>1673</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D35" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="E35" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="2">
         <v>1711</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D36" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="E36" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="2">
         <v>89</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D37" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="E37" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="2">
         <v>77</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="2">
         <v>79</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="2">
         <v>85</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="2">
         <v>1691</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="2">
         <v>1699</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="E42" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="2">
         <v>1701</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="E43" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="2">
         <v>1703</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="E44" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="2">
         <v>1705</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="2">
         <v>1707</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="E46" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="2">
         <v>87</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="E47" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="2">
         <v>1675</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="E48" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="2">
         <v>1677</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="E49" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="2">
         <v>1679</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="E50" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="2">
         <v>1681</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="E51" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="2">
         <v>1683</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="2">
         <v>1685</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>